<commit_message>
added more model variations
</commit_message>
<xml_diff>
--- a/drive_by_evaluation/results/results_summary.xlsx
+++ b/drive_by_evaluation/results/results_summary.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sw\master\code\drive-by-multi-lane-parking-detection-evaluation\drive_by_evaluation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{CABC4B39-12BE-4C46-9284-DC7DE791FE14}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54F4614-E43A-4930-9E87-53EB728A5574}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Dataset" sheetId="1" r:id="rId1"/>
-    <sheet name="Filtered Dataset" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="4" r:id="rId2"/>
+    <sheet name="Full Dataset - Less Features" sheetId="3" r:id="rId3"/>
+    <sheet name="Filtered Dataset" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
   <si>
     <t>Algorithmus</t>
   </si>
@@ -104,13 +106,19 @@
   </si>
   <si>
     <t>[[11717    93     1     0] [  453  1762     1     0] [  172    35     0     0] [   56    13     0     0]]</t>
+  </si>
+  <si>
+    <t>Recall Parking Car</t>
+  </si>
+  <si>
+    <t>Precision Parking Car</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,16 +134,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -172,11 +194,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -185,12 +246,154 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="11">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{D89C318D-A0D2-4185-B354-A37F8520101B}">
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -200,6 +403,78 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B9BEBB1-37A3-4981-9AA5-5829B69EE5C3}" name="Tabelle1" displayName="Tabelle1" ref="A2:L9" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="8">
+  <autoFilter ref="A2:L9" xr:uid="{9D5249F9-DB45-4217-AF00-00357AD17A5E}"/>
+  <sortState ref="A3:L9">
+    <sortCondition descending="1" ref="B2:B9"/>
+  </sortState>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{8B0125A7-2FEB-47AD-8D89-F8E97C4AE8C2}" name="Algorithmus" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{FBECA805-79C4-407D-A413-F5070498B313}" name="Accuracy"/>
+    <tableColumn id="3" xr3:uid="{BA3B32D2-81F1-4051-94E7-A8ED51C0AAD2}" name="FS Recall"/>
+    <tableColumn id="4" xr3:uid="{35D74497-0B4C-4706-8CFC-2CA79BC863FE}" name="FS Precision"/>
+    <tableColumn id="5" xr3:uid="{1CCEFDD2-13CC-4AA6-9B58-A3A2A74DF14B}" name="Recall Parking Car"/>
+    <tableColumn id="6" xr3:uid="{3DF16A8C-FD8A-4D3D-916D-C4A6C47CF42E}" name="Precision Parking Car"/>
+    <tableColumn id="7" xr3:uid="{09B35758-60B1-4A9F-A7AF-B490430F8A82}" name="OS Recall"/>
+    <tableColumn id="8" xr3:uid="{AE06A5B8-369D-4422-A9CE-27EA763E653C}" name="OS Precision"/>
+    <tableColumn id="9" xr3:uid="{EFDC8080-415F-43C4-8482-35486288AE9F}" name="OPV Recall"/>
+    <tableColumn id="10" xr3:uid="{6FD56D16-1D8F-4A93-8BE7-4B403F155663}" name="OPV Precision"/>
+    <tableColumn id="11" xr3:uid="{3358CEF6-5941-4339-9053-DC983CDE4E34}" name="Evaluation Time [s]"/>
+    <tableColumn id="12" xr3:uid="{2E141C2D-9EA1-4A46-BBE8-C1731F8B92C8}" name="Confusion-Matrix"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9285499F-2836-4F70-B52B-0D4D1910B7A1}" name="Tabelle14" displayName="Tabelle14" ref="A2:L9" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1">
+  <autoFilter ref="A2:L9" xr:uid="{A94372AB-13D6-4B57-A3D6-60B86C16CA4D}"/>
+  <sortState ref="A3:L9">
+    <sortCondition descending="1" ref="B2:B9"/>
+  </sortState>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{C8BE2C3C-CE32-4A77-BCC3-CC3A1C8BD74A}" name="Algorithmus" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{D3C77F9B-8C37-4F6E-B128-E5E97B28650C}" name="Accuracy"/>
+    <tableColumn id="3" xr3:uid="{89A801D5-10FE-42EE-8024-6C6418285B59}" name="FS Recall"/>
+    <tableColumn id="4" xr3:uid="{74366700-5E16-4D16-920C-A78EB0F91F79}" name="FS Precision"/>
+    <tableColumn id="5" xr3:uid="{DDDA42B0-8F30-4DC1-9494-2A338080F528}" name="PC Recall"/>
+    <tableColumn id="6" xr3:uid="{537789CF-70AB-4D6B-A1FE-6C240D655C59}" name="PC Precision"/>
+    <tableColumn id="7" xr3:uid="{5035664C-7F41-449F-BF4F-43C44FA7E58D}" name="OS Recall"/>
+    <tableColumn id="8" xr3:uid="{10AFED1D-8345-4758-BBFB-AB30C7D040E8}" name="OS Precision"/>
+    <tableColumn id="9" xr3:uid="{BF31B4F7-E61F-42BB-A67D-EAE5A9AC1CEE}" name="OPV Recall"/>
+    <tableColumn id="10" xr3:uid="{A3F0F2F6-C351-4AD2-AF66-02996784D5AE}" name="OPV Precision"/>
+    <tableColumn id="11" xr3:uid="{EC48FB30-A555-4A51-9AC2-2FD4588C27F9}" name="Evaluation Time [s]"/>
+    <tableColumn id="12" xr3:uid="{251204CF-5138-462A-8978-517FD2239BD2}" name="Confusion-Matrix"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{80BEB5E7-1F68-4020-B2D3-153152FB7CA0}" name="Tabelle13" displayName="Tabelle13" ref="A2:L9" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
+  <autoFilter ref="A2:L9" xr:uid="{B1627D82-E227-4704-A1B6-4B58C435E766}"/>
+  <sortState ref="A3:L9">
+    <sortCondition descending="1" ref="B2:B9"/>
+  </sortState>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{EDA529B8-4BA9-42EC-9A92-B6B7CAF5466B}" name="Algorithmus" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{CB6094BC-9F2F-41D9-ABF8-05C60A8D40D2}" name="Accuracy"/>
+    <tableColumn id="3" xr3:uid="{929F1B84-6757-476D-9474-08B768A4156A}" name="FS Recall"/>
+    <tableColumn id="4" xr3:uid="{72DE46C7-CFA3-46CD-890F-4731F93CF0FB}" name="FS Precision"/>
+    <tableColumn id="5" xr3:uid="{8D5B31F3-5BDA-4EE2-8520-EFA901EE1D3E}" name="PC Recall"/>
+    <tableColumn id="6" xr3:uid="{911586B3-F454-4A46-A2AA-82FCDB48BA6C}" name="PC Precision"/>
+    <tableColumn id="7" xr3:uid="{D53B8049-F9AC-45CF-B135-501BFAC90A8F}" name="OS Recall"/>
+    <tableColumn id="8" xr3:uid="{C11D16A2-309D-41B0-83B8-7A07C266C8A9}" name="OS Precision"/>
+    <tableColumn id="9" xr3:uid="{73B591E6-0904-4F14-9EBE-A7084278C7D8}" name="OPV Recall"/>
+    <tableColumn id="10" xr3:uid="{945C2102-7305-4ACF-8B7B-E4994EFCB5B5}" name="OPV Precision"/>
+    <tableColumn id="11" xr3:uid="{89C0F16C-6061-4639-8CDE-B8409B24CFD6}" name="Evaluation Time [s]"/>
+    <tableColumn id="12" xr3:uid="{4C9D6938-2D07-4EC0-82C0-10C7427EDCD2}" name="Confusion-Matrix"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -498,19 +773,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.140625" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
     <col min="12" max="12" width="85.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -528,10 +808,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>6</v>
@@ -594,66 +874,66 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>0.93448926798573695</v>
+        <v>0.94595539397329198</v>
       </c>
       <c r="C4">
-        <v>0.96714926999999995</v>
+        <v>0.98052662999999995</v>
       </c>
       <c r="D4">
-        <v>0.96961209000000004</v>
+        <v>0.96468138000000003</v>
       </c>
       <c r="E4">
-        <v>0.83935017999999995</v>
+        <v>0.86416968000000005</v>
       </c>
       <c r="F4">
-        <v>0.83633093999999997</v>
+        <v>0.86183617999999995</v>
       </c>
       <c r="G4">
-        <v>0.35748792000000001</v>
+        <v>0.14492753999999999</v>
       </c>
       <c r="H4">
-        <v>0.34418605000000002</v>
+        <v>0.44117646999999999</v>
       </c>
       <c r="I4">
-        <v>0.13043478</v>
+        <v>5.7971010000000003E-2</v>
       </c>
       <c r="J4">
-        <v>0.10843373000000001</v>
+        <v>0.5</v>
       </c>
       <c r="K4">
-        <v>9.2230536937713605</v>
+        <v>8.2165036201476997</v>
       </c>
       <c r="L4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>0.93847444592043605</v>
+        <v>0.94238970845277203</v>
       </c>
       <c r="C5">
-        <v>0.97697062000000001</v>
+        <v>0.99204132</v>
       </c>
       <c r="D5">
-        <v>0.96086269000000002</v>
+        <v>0.94507178999999997</v>
       </c>
       <c r="E5">
-        <v>0.83483755000000004</v>
+        <v>0.79512634999999998</v>
       </c>
       <c r="F5">
-        <v>0.83976395999999998</v>
+        <v>0.92590645999999999</v>
       </c>
       <c r="G5">
-        <v>0.16425121000000001</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.37362636999999999</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -662,162 +942,162 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>21.871115207672101</v>
+        <v>165.06024646758999</v>
       </c>
       <c r="L5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B6">
-        <v>0.49577011815702998</v>
+        <v>0.94141089281968804</v>
       </c>
       <c r="C6">
-        <v>0.42443484999999997</v>
+        <v>0.97764795999999998</v>
       </c>
       <c r="D6">
-        <v>0.98719968000000002</v>
+        <v>0.96104869000000004</v>
       </c>
       <c r="E6">
-        <v>0.87635379000000002</v>
+        <v>0.86146208999999996</v>
       </c>
       <c r="F6">
-        <v>0.46227088999999999</v>
+        <v>0.84059885999999995</v>
       </c>
       <c r="G6">
-        <v>0.38164250999999999</v>
+        <v>4.3478259999999998E-2</v>
       </c>
       <c r="H6">
-        <v>0.11002786000000001</v>
+        <v>0.52941176000000001</v>
       </c>
       <c r="I6">
-        <v>0.82608696000000004</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>1.323734E-2</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>7.5912740230560303</v>
+        <v>8.5402042865753103</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>0.94595539397329198</v>
+        <v>0.93847444592043605</v>
       </c>
       <c r="C7">
-        <v>0.98052662999999995</v>
+        <v>0.97697062000000001</v>
       </c>
       <c r="D7">
-        <v>0.96468138000000003</v>
+        <v>0.96086269000000002</v>
       </c>
       <c r="E7">
-        <v>0.86416968000000005</v>
+        <v>0.83483755000000004</v>
       </c>
       <c r="F7">
-        <v>0.86183617999999995</v>
+        <v>0.83976395999999998</v>
       </c>
       <c r="G7">
-        <v>0.14492753999999999</v>
+        <v>0.16425121000000001</v>
       </c>
       <c r="H7">
-        <v>0.44117646999999999</v>
+        <v>0.37362636999999999</v>
       </c>
       <c r="I7">
-        <v>5.7971010000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>8.2165036201476997</v>
+        <v>21.871115207672101</v>
       </c>
       <c r="L7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>0.94141089281968804</v>
+        <v>0.93448926798573695</v>
       </c>
       <c r="C8">
-        <v>0.97764795999999998</v>
+        <v>0.96714926999999995</v>
       </c>
       <c r="D8">
-        <v>0.96104869000000004</v>
+        <v>0.96961209000000004</v>
       </c>
       <c r="E8">
-        <v>0.86146208999999996</v>
+        <v>0.83935017999999995</v>
       </c>
       <c r="F8">
-        <v>0.84059885999999995</v>
+        <v>0.83633093999999997</v>
       </c>
       <c r="G8">
-        <v>4.3478259999999998E-2</v>
+        <v>0.35748792000000001</v>
       </c>
       <c r="H8">
-        <v>0.52941176000000001</v>
+        <v>0.34418605000000002</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>0.13043478</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>0.10843373000000001</v>
       </c>
       <c r="K8">
-        <v>8.5402042865753103</v>
+        <v>9.2230536937713605</v>
       </c>
       <c r="L8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>0.94238970845277203</v>
+        <v>0.49577011815702998</v>
       </c>
       <c r="C9">
-        <v>0.99204132</v>
+        <v>0.42443484999999997</v>
       </c>
       <c r="D9">
-        <v>0.94507178999999997</v>
+        <v>0.98719968000000002</v>
       </c>
       <c r="E9">
-        <v>0.79512634999999998</v>
+        <v>0.87635379000000002</v>
       </c>
       <c r="F9">
-        <v>0.92590645999999999</v>
+        <v>0.46227088999999999</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.38164250999999999</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.11002786000000001</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>0.82608696000000004</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1.323734E-2</v>
       </c>
       <c r="K9">
-        <v>165.06024646758999</v>
+        <v>7.5912740230560303</v>
       </c>
       <c r="L9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -850,17 +1130,284 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB9D49D-3D63-405E-BE5F-7E287444A72C}">
+  <dimension ref="A4:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="5" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC73976-D93E-4C2C-A1E2-377B96FE27DE}">
+  <dimension ref="A2:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="71" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>30.116367578506399</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="71" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added results + fixed deep learning evaluation
</commit_message>
<xml_diff>
--- a/drive_by_evaluation/results/results_summary.xlsx
+++ b/drive_by_evaluation/results/results_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sw\master\code\drive-by-multi-lane-parking-detection-evaluation\drive_by_evaluation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D687D1-EE43-48FA-9711-4F4D9ABA04BE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C624F8A8-239B-448D-8977-B0F4A6BFB15E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="254">
   <si>
     <t>Algorithmus</t>
   </si>
@@ -757,6 +757,36 @@
   </si>
   <si>
     <t>[[6489 177 4 10 ][282 1865 24 12 ][17 33 16 0 ][36 12 1 11 ]]</t>
+  </si>
+  <si>
+    <t>dense_5layer32_dropout20_epochs200</t>
+  </si>
+  <si>
+    <t>full_dataset_raw_sensor_10cm</t>
+  </si>
+  <si>
+    <t>[[11420 381 10 0 ][289 1916 11 0 ][52 123 32 0 ][47 22 0 0 ]]</t>
+  </si>
+  <si>
+    <t>[[6267 413 0 0 ][177 1998 8 0 ][11 44 11 0 ][35 25 0 0 ]]</t>
+  </si>
+  <si>
+    <t>[[8264 1154 537 1856 ][88 1760 284 84 ][17 90 81 19 ][6 12 5 46 ]]</t>
+  </si>
+  <si>
+    <t>[[5283 614 188 595 ][116 1891 98 78 ][7 27 28 4 ][6 9 8 37 ]]</t>
+  </si>
+  <si>
+    <t>[[3427 3358 676 4350 ][3 1771 112 330 ][5 83 66 53 ][1 4 0 64 ]]</t>
+  </si>
+  <si>
+    <t>[[2109 2095 256 2220 ][8 1458 399 318 ][0 12 36 18 ][1 2 2 55 ]]</t>
+  </si>
+  <si>
+    <t>[[8814 837 373 1787 ][145 1730 262 79 ][22 88 80 17 ][9 8 4 48 ]]</t>
+  </si>
+  <si>
+    <t>[[5356 474 167 683 ][146 1855 100 82 ][7 29 24 6 ][7 8 7 38 ]]</t>
   </si>
 </sst>
 </file>
@@ -932,8 +962,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0C681CE7-729A-45E9-898E-3542B03C5255}" name="Tabelle4" displayName="Tabelle4" ref="A4:R325" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A4:R325" xr:uid="{4260E9C2-4E25-4618-8142-7E009B061F1A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0C681CE7-729A-45E9-898E-3542B03C5255}" name="Tabelle4" displayName="Tabelle4" ref="A4:R333" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A4:R333" xr:uid="{4260E9C2-4E25-4618-8142-7E009B061F1A}"/>
   <sortState ref="A5:R325">
     <sortCondition descending="1" ref="L4:L325"/>
   </sortState>
@@ -1260,10 +1290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB9D49D-3D63-405E-BE5F-7E287444A72C}">
-  <dimension ref="A4:R325"/>
+  <dimension ref="A4:R333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
+      <selection activeCell="L335" sqref="L335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19637,6 +19667,462 @@
         <v>168</v>
       </c>
     </row>
+    <row r="326" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>244</v>
+      </c>
+      <c r="B326" t="s">
+        <v>245</v>
+      </c>
+      <c r="C326" t="s">
+        <v>14</v>
+      </c>
+      <c r="D326">
+        <v>10</v>
+      </c>
+      <c r="E326" t="s">
+        <v>15</v>
+      </c>
+      <c r="F326" t="s">
+        <v>141</v>
+      </c>
+      <c r="G326">
+        <v>0.93462909879046296</v>
+      </c>
+      <c r="H326">
+        <v>0.96689526712386697</v>
+      </c>
+      <c r="I326">
+        <v>0.96714092140921404</v>
+      </c>
+      <c r="J326">
+        <v>0.86462093862815803</v>
+      </c>
+      <c r="K326">
+        <v>0.78460278460278399</v>
+      </c>
+      <c r="L326">
+        <f>2*(Tabelle4[[#This Row],[Precision Parking Car]]*Tabelle4[[#This Row],[Recall Parking Car]])/(Tabelle4[[#This Row],[Precision Parking Car]]+Tabelle4[[#This Row],[Recall Parking Car]])</f>
+        <v>0.82267067410905903</v>
+      </c>
+      <c r="M326" s="4">
+        <v>0.15458937198067599</v>
+      </c>
+      <c r="N326">
+        <v>0.60377358490566002</v>
+      </c>
+      <c r="O326">
+        <v>0</v>
+      </c>
+      <c r="P326" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q326">
+        <v>2103.03870868682</v>
+      </c>
+      <c r="R326" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="327" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>244</v>
+      </c>
+      <c r="B327" t="s">
+        <v>242</v>
+      </c>
+      <c r="C327" t="s">
+        <v>14</v>
+      </c>
+      <c r="D327">
+        <v>10</v>
+      </c>
+      <c r="E327" t="s">
+        <v>15</v>
+      </c>
+      <c r="F327" t="s">
+        <v>141</v>
+      </c>
+      <c r="G327">
+        <v>0.92068083212815599</v>
+      </c>
+      <c r="H327">
+        <v>0.93817365269460995</v>
+      </c>
+      <c r="I327">
+        <v>0.96563944530046197</v>
+      </c>
+      <c r="J327">
+        <v>0.91525423728813504</v>
+      </c>
+      <c r="K327">
+        <v>0.80564516129032204</v>
+      </c>
+      <c r="L327">
+        <f>2*(Tabelle4[[#This Row],[Precision Parking Car]]*Tabelle4[[#This Row],[Recall Parking Car]])/(Tabelle4[[#This Row],[Precision Parking Car]]+Tabelle4[[#This Row],[Recall Parking Car]])</f>
+        <v>0.85695903924512062</v>
+      </c>
+      <c r="M327" s="4">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="N327">
+        <v>0.57894736842105199</v>
+      </c>
+      <c r="O327">
+        <v>0</v>
+      </c>
+      <c r="P327" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q327">
+        <v>1736.1670012474001</v>
+      </c>
+      <c r="R327" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="328" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>244</v>
+      </c>
+      <c r="B328" t="s">
+        <v>245</v>
+      </c>
+      <c r="C328" t="s">
+        <v>14</v>
+      </c>
+      <c r="D328">
+        <v>10</v>
+      </c>
+      <c r="E328" t="s">
+        <v>15</v>
+      </c>
+      <c r="F328" t="s">
+        <v>140</v>
+      </c>
+      <c r="G328">
+        <v>0.70971124938824004</v>
+      </c>
+      <c r="H328">
+        <v>0.69968673270679804</v>
+      </c>
+      <c r="I328">
+        <v>0.986746268656716</v>
+      </c>
+      <c r="J328">
+        <v>0.79422382671480096</v>
+      </c>
+      <c r="K328">
+        <v>0.58355437665782495</v>
+      </c>
+      <c r="L328">
+        <f>2*(Tabelle4[[#This Row],[Precision Parking Car]]*Tabelle4[[#This Row],[Recall Parking Car]])/(Tabelle4[[#This Row],[Precision Parking Car]]+Tabelle4[[#This Row],[Recall Parking Car]])</f>
+        <v>0.67278287461773678</v>
+      </c>
+      <c r="M328" s="4">
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="N328">
+        <v>8.93054024255788E-2</v>
+      </c>
+      <c r="O328">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="P328">
+        <v>2.2942643391521099E-2</v>
+      </c>
+      <c r="Q328">
+        <v>6942.5407080650302</v>
+      </c>
+      <c r="R328" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="329" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>244</v>
+      </c>
+      <c r="B329" t="s">
+        <v>242</v>
+      </c>
+      <c r="C329" t="s">
+        <v>14</v>
+      </c>
+      <c r="D329">
+        <v>10</v>
+      </c>
+      <c r="E329" t="s">
+        <v>15</v>
+      </c>
+      <c r="F329" t="s">
+        <v>140</v>
+      </c>
+      <c r="G329">
+        <v>0.80531761041272598</v>
+      </c>
+      <c r="H329">
+        <v>0.79086826347305395</v>
+      </c>
+      <c r="I329">
+        <v>0.97616407982261599</v>
+      </c>
+      <c r="J329">
+        <v>0.86623912047640805</v>
+      </c>
+      <c r="K329">
+        <v>0.74419519874065299</v>
+      </c>
+      <c r="L329">
+        <f>2*(Tabelle4[[#This Row],[Precision Parking Car]]*Tabelle4[[#This Row],[Recall Parking Car]])/(Tabelle4[[#This Row],[Precision Parking Car]]+Tabelle4[[#This Row],[Recall Parking Car]])</f>
+        <v>0.80059271803556276</v>
+      </c>
+      <c r="M329" s="4">
+        <v>0.42424242424242398</v>
+      </c>
+      <c r="N329">
+        <v>8.6956521739130405E-2</v>
+      </c>
+      <c r="O329">
+        <v>0.61666666666666603</v>
+      </c>
+      <c r="P329">
+        <v>5.1820728291316502E-2</v>
+      </c>
+      <c r="Q329">
+        <v>4156.3238830566397</v>
+      </c>
+      <c r="R329" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="330" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>244</v>
+      </c>
+      <c r="B330" t="s">
+        <v>245</v>
+      </c>
+      <c r="C330" t="s">
+        <v>14</v>
+      </c>
+      <c r="D330">
+        <v>10</v>
+      </c>
+      <c r="E330" t="s">
+        <v>15</v>
+      </c>
+      <c r="F330" t="s">
+        <v>143</v>
+      </c>
+      <c r="G330">
+        <v>0.37250926379081301</v>
+      </c>
+      <c r="H330">
+        <v>0.29015324697315997</v>
+      </c>
+      <c r="I330">
+        <v>0.99738067520372498</v>
+      </c>
+      <c r="J330">
+        <v>0.79918772563176899</v>
+      </c>
+      <c r="K330">
+        <v>0.339532208588957</v>
+      </c>
+      <c r="L330">
+        <f>2*(Tabelle4[[#This Row],[Precision Parking Car]]*Tabelle4[[#This Row],[Recall Parking Car]])/(Tabelle4[[#This Row],[Precision Parking Car]]+Tabelle4[[#This Row],[Recall Parking Car]])</f>
+        <v>0.47658772874058125</v>
+      </c>
+      <c r="M330" s="4">
+        <v>0.31884057971014401</v>
+      </c>
+      <c r="N330">
+        <v>7.7283372365339498E-2</v>
+      </c>
+      <c r="O330">
+        <v>0.92753623188405798</v>
+      </c>
+      <c r="P330">
+        <v>1.3341671878257201E-2</v>
+      </c>
+      <c r="Q330">
+        <v>231.124272823333</v>
+      </c>
+      <c r="R330" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="331" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>244</v>
+      </c>
+      <c r="B331" t="s">
+        <v>242</v>
+      </c>
+      <c r="C331" t="s">
+        <v>14</v>
+      </c>
+      <c r="D331">
+        <v>10</v>
+      </c>
+      <c r="E331" t="s">
+        <v>15</v>
+      </c>
+      <c r="F331" t="s">
+        <v>143</v>
+      </c>
+      <c r="G331">
+        <v>0.406941817777283</v>
+      </c>
+      <c r="H331">
+        <v>0.31571856287425099</v>
+      </c>
+      <c r="I331">
+        <v>0.99575070821529699</v>
+      </c>
+      <c r="J331">
+        <v>0.66788822721026098</v>
+      </c>
+      <c r="K331">
+        <v>0.40874684608915002</v>
+      </c>
+      <c r="L331">
+        <f>2*(Tabelle4[[#This Row],[Precision Parking Car]]*Tabelle4[[#This Row],[Recall Parking Car]])/(Tabelle4[[#This Row],[Precision Parking Car]]+Tabelle4[[#This Row],[Recall Parking Car]])</f>
+        <v>0.50713043478260833</v>
+      </c>
+      <c r="M331" s="4">
+        <v>0.54545454545454497</v>
+      </c>
+      <c r="N331">
+        <v>5.1948051948051903E-2</v>
+      </c>
+      <c r="O331">
+        <v>0.91666666666666596</v>
+      </c>
+      <c r="P331">
+        <v>2.10647261585599E-2</v>
+      </c>
+      <c r="Q331">
+        <v>177.114655494689</v>
+      </c>
+      <c r="R331" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="332" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>244</v>
+      </c>
+      <c r="B332" t="s">
+        <v>245</v>
+      </c>
+      <c r="C332" t="s">
+        <v>14</v>
+      </c>
+      <c r="D332">
+        <v>10</v>
+      </c>
+      <c r="E332" t="s">
+        <v>15</v>
+      </c>
+      <c r="F332" t="s">
+        <v>192</v>
+      </c>
+      <c r="G332">
+        <v>0.74613717401943602</v>
+      </c>
+      <c r="H332">
+        <v>0.74625349250698503</v>
+      </c>
+      <c r="I332">
+        <v>0.98042269187986597</v>
+      </c>
+      <c r="J332">
+        <v>0.78068592057761699</v>
+      </c>
+      <c r="K332">
+        <v>0.64964325948178703</v>
+      </c>
+      <c r="L332">
+        <f>2*(Tabelle4[[#This Row],[Precision Parking Car]]*Tabelle4[[#This Row],[Recall Parking Car]])/(Tabelle4[[#This Row],[Precision Parking Car]]+Tabelle4[[#This Row],[Recall Parking Car]])</f>
+        <v>0.70916171346587364</v>
+      </c>
+      <c r="M332" s="4">
+        <v>0.38647342995168998</v>
+      </c>
+      <c r="N332">
+        <v>0.11126564673157099</v>
+      </c>
+      <c r="O332">
+        <v>0.69565217391304301</v>
+      </c>
+      <c r="P332">
+        <v>2.48575867426204E-2</v>
+      </c>
+      <c r="Q332">
+        <v>10763.885279893801</v>
+      </c>
+      <c r="R332" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="333" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>244</v>
+      </c>
+      <c r="B333" t="s">
+        <v>242</v>
+      </c>
+      <c r="C333" t="s">
+        <v>14</v>
+      </c>
+      <c r="D333">
+        <v>10</v>
+      </c>
+      <c r="E333" t="s">
+        <v>15</v>
+      </c>
+      <c r="F333" t="s">
+        <v>192</v>
+      </c>
+      <c r="G333">
+        <v>0.80910001112470797</v>
+      </c>
+      <c r="H333">
+        <v>0.80179640718562795</v>
+      </c>
+      <c r="I333">
+        <v>0.97099347353154397</v>
+      </c>
+      <c r="J333">
+        <v>0.84974805313788304</v>
+      </c>
+      <c r="K333">
+        <v>0.78402366863905304</v>
+      </c>
+      <c r="L333">
+        <f>2*(Tabelle4[[#This Row],[Precision Parking Car]]*Tabelle4[[#This Row],[Recall Parking Car]])/(Tabelle4[[#This Row],[Precision Parking Car]]+Tabelle4[[#This Row],[Recall Parking Car]])</f>
+        <v>0.81556386018905214</v>
+      </c>
+      <c r="M333" s="4">
+        <v>0.36363636363636298</v>
+      </c>
+      <c r="N333">
+        <v>8.0536912751677805E-2</v>
+      </c>
+      <c r="O333">
+        <v>0.63333333333333297</v>
+      </c>
+      <c r="P333">
+        <v>4.6971569839307697E-2</v>
+      </c>
+      <c r="Q333">
+        <v>6253.40963196754</v>
+      </c>
+      <c r="R333" t="s">
+        <v>253</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>